<commit_message>
Improved Printer and Parser
</commit_message>
<xml_diff>
--- a/Tensor products.xlsx
+++ b/Tensor products.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Eclipse\WorkSpace\calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joepg\Dropbox\Eclipse\WorkSpace\calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D5597DE9-8851-46AD-BFA9-099BA1C7CD87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E70EDD2-A085-48A9-9066-695879F0BA4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{5C809F79-D9A1-4D1B-B26E-8D80F0ED876A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6930" xr2:uid="{5C809F79-D9A1-4D1B-B26E-8D80F0ED876A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
   <si>
     <t>Object a</t>
   </si>
@@ -141,15 +136,49 @@
   </si>
   <si>
     <t>Matrix product</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Derivatives</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>variable shape</t>
+  </si>
+  <si>
+    <t>Deriving with respect to</t>
+  </si>
+  <si>
+    <t>normal function'</t>
+  </si>
+  <si>
+    <t>multivariate scalar function</t>
+  </si>
+  <si>
+    <t>vector function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -176,10 +205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -496,99 +528,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796D13E6-4A5C-40C6-BA70-AAED31A05BD4}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="M1" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="M2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -599,28 +619,25 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -631,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -649,39 +666,42 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -692,10 +712,10 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -703,14 +723,14 @@
       <c r="I7" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>11</v>
       </c>
       <c r="M7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -721,126 +741,268 @@
         <v>16</v>
       </c>
       <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>21</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>22</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>35</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>15</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>34</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>33</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>